<commit_message>
add extension methods, update export templates.
</commit_message>
<xml_diff>
--- a/Source/GraduateThesisManagement/GraduateThesis.Web/wwwroot/reports/faculty-staff_export.xlsx
+++ b/Source/GraduateThesisManagement/GraduateThesis.Web/wwwroot/reports/faculty-staff_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HUFI_GRADUATE-THESIS\HUFI_graduate-thesis-management\Source\GraduateThesisManagement\GraduateThesis.Web\wwwroot\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C780C24-B20E-4AF1-8EE4-9D01AA3F5BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8AC5AC-4AEE-496D-B10F-FA50BEF8466F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9618D36F-91D3-4472-B248-079CF11FD3FC}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>{{Items.Surname}}</t>
   </si>
   <si>
-    <t>DANH SÁCH GIẢNG VIÊN CỦA KHOA CÔNG NGHỆ THÔNG TIN</t>
-  </si>
-  <si>
     <t>{{Items.Id}}</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>{{Items.Birthday}}</t>
+  </si>
+  <si>
+    <t>{{Name}}</t>
   </si>
 </sst>
 </file>
@@ -195,19 +195,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +527,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -542,14 +542,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.6" customHeight="1" thickBot="1">
-      <c r="A1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="22.2" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -558,10 +558,10 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
@@ -574,23 +574,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>